<commit_message>
change names of sample files.
</commit_message>
<xml_diff>
--- a/data/data_set_samples/abuse/cell_list.xlsx
+++ b/data/data_set_samples/abuse/cell_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vdeange\Documents\BA\battery_archive_demo\all_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vdeange\PycharmProjects\battery-archive-sandbox\data\data_set_samples\abuse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6D081B-5C0F-475D-8892-90A9B57B5405}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{138E6542-C88A-40C9-A5E6-9CF3B4FB9A9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1665" windowWidth="26955" windowHeight="11385" xr2:uid="{07EF3D65-9BA3-43DB-B014-0F8C59FBB292}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{07EF3D65-9BA3-43DB-B014-0F8C59FBB292}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -83,24 +83,12 @@
     <t>thickness</t>
   </si>
   <si>
-    <t>ChevyVolt-100SOC-6mm-cell4_ORNL</t>
-  </si>
-  <si>
-    <t>ORNL_1</t>
-  </si>
-  <si>
     <t>pouch</t>
   </si>
   <si>
     <t>xlsx</t>
   </si>
   <si>
-    <t>NMC-LMO_Graphite_26Ah_100SOC_Test1_SNL</t>
-  </si>
-  <si>
-    <t>SNL_1</t>
-  </si>
-  <si>
     <t>snl</t>
   </si>
   <si>
@@ -114,6 +102,18 @@
   </si>
   <si>
     <t>nail_speed</t>
+  </si>
+  <si>
+    <t>sample_2</t>
+  </si>
+  <si>
+    <t>S2Abuse</t>
+  </si>
+  <si>
+    <t>S1Abuse</t>
+  </si>
+  <si>
+    <t>sample_1</t>
   </si>
 </sst>
 </file>
@@ -506,7 +506,7 @@
   <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,13 +554,13 @@
         <v>15</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>11</v>
@@ -575,10 +575,10 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>0</v>
@@ -593,7 +593,7 @@
         <v>26</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H2" s="3">
         <v>25</v>
@@ -611,21 +611,21 @@
         <v>0.05</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>0</v>
@@ -640,7 +640,7 @@
         <v>26</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H3" s="3">
         <v>25</v>
@@ -658,13 +658,13 @@
         <v>0.05</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>